<commit_message>
Added product category and products
</commit_message>
<xml_diff>
--- a/Resources/UserRolePermissionMapping.xlsx
+++ b/Resources/UserRolePermissionMapping.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code Bases\RetailCoreSolution\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A7F114-77B5-4473-888E-F6241C66B268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DE0BF4-EA3F-4863-A0BF-D8A20ED41819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{14AE3CD4-92AB-41CB-A3B8-04D95F14FDBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="5" xr2:uid="{14AE3CD4-92AB-41CB-A3B8-04D95F14FDBD}"/>
   </bookViews>
   <sheets>
     <sheet name="User Role Permission" sheetId="1" r:id="rId1"/>
-    <sheet name="Role Levels" sheetId="2" r:id="rId2"/>
-    <sheet name="Roles" sheetId="3" r:id="rId3"/>
+    <sheet name="Roles" sheetId="3" r:id="rId2"/>
+    <sheet name="Role Levels" sheetId="2" r:id="rId3"/>
     <sheet name="Permission Types" sheetId="4" r:id="rId4"/>
     <sheet name="Permissions" sheetId="5" r:id="rId5"/>
     <sheet name="Role Level Permission Types" sheetId="6" r:id="rId6"/>
@@ -130,9 +130,6 @@
     <t>Add Product</t>
   </si>
   <si>
-    <t>Edit Product:</t>
-  </si>
-  <si>
     <t>Delete Product</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t>Permission</t>
+  </si>
+  <si>
+    <t>Edit Product</t>
   </si>
 </sst>
 </file>
@@ -300,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -312,9 +312,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -440,7 +437,7 @@
                   <a14:compatExt spid="_x0000_s6152"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{218D4F65-212D-E804-DF06-9E1F26DC46B9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -498,7 +495,7 @@
                   <a14:compatExt spid="_x0000_s6159"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F061895-19D3-B01A-6F40-6D06525F516A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -556,7 +553,7 @@
                   <a14:compatExt spid="_x0000_s6160"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE05A6C8-8CFB-DC20-E123-246DEF2477C6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -614,7 +611,7 @@
                   <a14:compatExt spid="_x0000_s6161"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D9D8CD2-0E51-0E64-BDE7-3612522B62CE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -672,7 +669,7 @@
                   <a14:compatExt spid="_x0000_s6163"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C4BB23F-9710-7071-6B44-8F4E311767E9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -711,34 +708,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BB056611-2887-4FCA-A631-EBC718DF52A1}" name="Table3" displayName="Table3" ref="C1:D9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="C1:D9" xr:uid="{BB056611-2887-4FCA-A631-EBC718DF52A1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{59EBE738-E30B-4412-95C9-08B69ADB9C3E}" name="Role" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{3BE4F590-C638-4BC0-8412-60FB4DCC9724}" name="Role Level" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B799D596-965E-459B-B588-2935C1C91200}" name="Table2" displayName="Table2" ref="B1:D6" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" dataCellStyle="Normal">
   <autoFilter ref="B1:D6" xr:uid="{B799D596-965E-459B-B588-2935C1C91200}"/>
   <tableColumns count="3">
     <tableColumn id="2" xr3:uid="{F8E0FBF9-D3A3-4C76-AC4D-1766740E2611}" name="Sr Number" dataDxfId="16" dataCellStyle="Normal"/>
     <tableColumn id="1" xr3:uid="{D048790D-FDFB-4E43-8CA0-20542F132BB8}" name="ROLE LEVEL NAME" dataDxfId="15" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{A6EBED66-71B5-4DEC-9245-9054BC804CF2}" name="ROLE LEVEL" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{A6EBED66-71B5-4DEC-9245-9054BC804CF2}" name="ROLE LEVEL" dataDxfId="14" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BB056611-2887-4FCA-A631-EBC718DF52A1}" name="Table3" displayName="Table3" ref="C1:D9" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="C1:D9" xr:uid="{BB056611-2887-4FCA-A631-EBC718DF52A1}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{59EBE738-E30B-4412-95C9-08B69ADB9C3E}" name="Role" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{3BE4F590-C638-4BC0-8412-60FB4DCC9724}" name="Role Level" dataDxfId="11"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B42B2027-F156-4C16-803D-271C31C21025}" name="Table4" displayName="Table4" ref="B1:C8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B42B2027-F156-4C16-803D-271C31C21025}" name="Table4" displayName="Table4" ref="B1:C8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="B1:C8" xr:uid="{B42B2027-F156-4C16-803D-271C31C21025}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BCC991AB-DF01-4741-A4CC-93D42DF799D3}" name="Sr Number" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{76FA6F78-AF46-41A3-B052-602F6A666EBB}" name="Permission Types" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{BCC991AB-DF01-4741-A4CC-93D42DF799D3}" name="Sr Number" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{76FA6F78-AF46-41A3-B052-602F6A666EBB}" name="Permission Types" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -757,11 +754,11 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3979C7AC-8BF6-443E-A3F4-C88FDC5ACBBD}" name="Table7" displayName="Table7" ref="B1:E6" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3979C7AC-8BF6-443E-A3F4-C88FDC5ACBBD}" name="Table7" displayName="Table7" ref="B1:E6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="B1:E6" xr:uid="{3979C7AC-8BF6-443E-A3F4-C88FDC5ACBBD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7FA7D991-86EF-403F-8BD5-14CF6D7527F5}" name="Sr Number" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{DB7E11DB-4ED6-42C1-A8F3-9E50D88F4790}" name="ROLE LEVEL" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{7FA7D991-86EF-403F-8BD5-14CF6D7527F5}" name="Sr Number" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{DB7E11DB-4ED6-42C1-A8F3-9E50D88F4790}" name="ROLE LEVEL" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{A8EBA54C-D960-440A-8A01-746CEFCBC5E5}" name="PERMISSION TYPE" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{7A82B49F-FB96-4FB1-9622-30D15353A22D}" name="Remarks" dataDxfId="0"/>
   </tableColumns>
@@ -1088,7 +1085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F5C6AF-479F-47DB-BB4A-92140CEB2B58}">
   <dimension ref="B4:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1102,13 +1099,13 @@
   <sheetData>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1117,95 +1114,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81354C0F-F5B3-47B1-9490-07CF28DC75DA}">
-  <dimension ref="B1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="5">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="5">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06FC1BB-9BB0-498B-BE63-EBFB40CE617C}">
   <dimension ref="B1:D9"/>
   <sheetViews>
@@ -1340,12 +1248,101 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81354C0F-F5B3-47B1-9490-07CF28DC75DA}">
+  <dimension ref="B1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D7A950-E63F-4FD6-80C0-9890B268A003}">
   <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -1431,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D0E648-C6C2-46C3-AA45-7F1D14117B61}">
   <dimension ref="B1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,13 +1441,13 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -1458,10 +1455,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -1469,10 +1466,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1557,7 +1554,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -1568,7 +1565,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -1579,7 +1576,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -1590,7 +1587,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -1601,7 +1598,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -1612,7 +1609,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -1623,7 +1620,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -1634,7 +1631,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -1645,7 +1642,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -1656,7 +1653,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
@@ -1667,7 +1664,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
@@ -1678,7 +1675,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -1689,7 +1686,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
@@ -1700,7 +1697,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
@@ -1711,7 +1708,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -1722,7 +1719,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -1733,7 +1730,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -1744,7 +1741,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -1757,18 +1754,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{67A84D7B-9E57-4343-8422-9373B27B1AC1}">
           <x14:formula1>
             <xm:f>'Permission Types'!$C$2:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D4:D28</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4536D174-5B51-4D55-A724-62F2A5AA6041}">
-          <x14:formula1>
-            <xm:f>'Permission Types'!$C$2:$C$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D3</xm:sqref>
+          <xm:sqref>D2:D28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1780,7 +1771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691E0375-7912-497A-87DB-77FC865D765D}">
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1800,10 +1791,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1814,8 +1805,8 @@
         <v>11</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="6" t="s">
-        <v>54</v>
+      <c r="E2" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1826,8 +1817,8 @@
         <v>12</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="6" t="s">
-        <v>59</v>
+      <c r="E3" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1838,8 +1829,8 @@
         <v>19</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="6" t="s">
-        <v>58</v>
+      <c r="E4" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -1850,8 +1841,8 @@
         <v>20</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="6" t="s">
-        <v>56</v>
+      <c r="E5" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1862,8 +1853,8 @@
         <v>21</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="6" t="s">
-        <v>57</v>
+      <c r="E6" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>